<commit_message>
includes bc replacements sheet
</commit_message>
<xml_diff>
--- a/xlsx/hfc_replacements.xlsx
+++ b/xlsx/hfc_replacements.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Box Sync\GitHub\high-frequency-checks\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Box Sync\GitHub\dmsetup\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,13 +13,14 @@
   </bookViews>
   <sheets>
     <sheet name="hfc_replacements" sheetId="1" r:id="rId1"/>
+    <sheet name="bc_replacements" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
   <si>
     <t>newvalue</t>
   </si>
@@ -49,6 +50,12 @@
   </si>
   <si>
     <t>action</t>
+  </si>
+  <si>
+    <t>bcer_id</t>
+  </si>
+  <si>
+    <t>bcer_name</t>
   </si>
 </sst>
 </file>
@@ -102,7 +109,47 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color theme="0" tint="-0.499984740745262"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.499984740745262"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.499984740745262"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.499984740745262"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -877,6 +924,780 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="11039475" y="8048625"/>
+          <a:ext cx="3667125" cy="676275"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t>dropping observations</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
+            <a:t>To drop an entire observation, specify the surveyid (eg. hhid, employee_id) and specify -333 in the newvalue column </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE715E01-8487-486B-B777-DDA92557CD65}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13201650" y="47625"/>
+          <a:ext cx="3648075" cy="2895600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" u="sng"/>
+            <a:t>BC Replacements and Corrections</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="1" baseline="0"/>
+            <a:t>This file keeps a running list of replacements/corrections that are made to the raw data set during data collection. It is designed to be read by the </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" i="1" baseline="0"/>
+            <a:t>ipacheckreadreplace</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="1" baseline="0"/>
+            <a:t> command in the </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" i="1" baseline="0"/>
+            <a:t>master_check.do</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="1" baseline="0"/>
+            <a:t> file. You'll notice that it shares the same format with the HFC output. The expected workflow is:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="1" baseline="0"/>
+            <a:t>   1. A problem is identified by the HFC commands and </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="1" baseline="0"/>
+            <a:t>       included in the output file.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="1" baseline="0"/>
+            <a:t>   2. After tracking by the RA and field team a solution is </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="1" baseline="0"/>
+            <a:t>       discovered.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="1" baseline="0"/>
+            <a:t>    3. If necessary, a replacement value is recorded in the </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="1" baseline="0"/>
+            <a:t>        replacements file (here) or the observation may be </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="1" baseline="0"/>
+            <a:t>        marked to be dropped.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="1" baseline="0"/>
+            <a:t>    4. HFCs are re-run incorporating the changes in the </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="1" baseline="0"/>
+            <a:t>        replacements file. If the observation is now valid</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="1" baseline="0"/>
+            <a:t>        it will no longer appear in the output.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" b="0" i="1" baseline="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1BFBAE69-139B-43BA-BD1E-57917DD39213}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13201650" y="5114925"/>
+          <a:ext cx="3667125" cy="609600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="92D050"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t>variable</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
+            <a:t>This column specifies the variable within the observation whose value will be dropped or replaced.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="TextBox 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B5D8ED0-5C5C-42F8-92F4-432A26C6B809}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13192125" y="3000375"/>
+          <a:ext cx="3667125" cy="628650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="92D050"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t>date</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
+            <a:t>This column specifies the date the replacement was entered into this correction sheet</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="TextBox 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D2D05618-A3FE-4D1D-A33E-D691CE6EFF79}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13201650" y="3686175"/>
+          <a:ext cx="3667125" cy="628650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="92D050"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t>skey</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
+            <a:t>This column specifies the skey of the observation to be dropped or replaced. </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>152399</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>47624</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="TextBox 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{568DF475-0BD4-4FD3-BBC6-066ED280BCE7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13201650" y="4381499"/>
+          <a:ext cx="3667125" cy="657225"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="92D050"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t>bcer_id and bcer_name</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
+            <a:t>These columns specified enumerator details for the observation</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="TextBox 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{52BB89B2-4747-4751-A463-60C3645A5F34}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13201650" y="5800725"/>
+          <a:ext cx="3667125" cy="609600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="92D050"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t>value</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
+            <a:t>This column specifies the current value that will be replaced in the survey data set.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="TextBox 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE0B58CE-1003-433A-9D69-FA9398209E9D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13201650" y="6467475"/>
+          <a:ext cx="3667125" cy="609600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="92D050"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t>newvalue</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
+            <a:t>This column specifies the new value that will be placed in the survey data set.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>66674</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="TextBox 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F23F4708-8668-496F-B4A0-A834FA0AE525}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13201650" y="7153274"/>
+          <a:ext cx="3667125" cy="838201"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FF0000"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t>dropping values</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
+            <a:t>To drop the value of a particular variable, specify the variable under the variable column and leave the newvalue column blank</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="TextBox 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5B50EC2D-2CC5-45F7-83E3-F78DB73D7A8A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13192125" y="8048625"/>
           <a:ext cx="3667125" cy="676275"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1233,7 +2054,7 @@
       <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomRight" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1312,17 +2133,124 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:J1048576">
+    <cfRule type="expression" dxfId="5" priority="1">
+      <formula>$A1&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:XFD1">
+    <cfRule type="expression" dxfId="4" priority="3">
+      <formula>A$1&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J1">
+    <cfRule type="expression" dxfId="3" priority="6">
+      <formula>K$1&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K9"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <pane xSplit="5" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F1" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="J27" sqref="J27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="15.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" customWidth="1"/>
+    <col min="6" max="6" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" customWidth="1"/>
+    <col min="9" max="9" width="14.85546875" customWidth="1"/>
+    <col min="10" max="10" width="35.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="18" customHeight="1">
+      <c r="A1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1"/>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="5"/>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="5"/>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="5"/>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="5"/>
+      <c r="G5" s="6"/>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="5"/>
+      <c r="G6" s="6"/>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="5"/>
+      <c r="G7" s="6"/>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="G8" s="6"/>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="G9" s="6"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A1:J1048576">
     <cfRule type="expression" dxfId="2" priority="1">
       <formula>$A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:XFD1">
-    <cfRule type="expression" dxfId="1" priority="3">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>A$1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1">
-    <cfRule type="expression" dxfId="0" priority="6">
+    <cfRule type="expression" dxfId="0" priority="3">
       <formula>K$1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>